<commit_message>
Add: data karyawan tempat tanggal lahir, golongan darah, status pernikahan
</commit_message>
<xml_diff>
--- a/public/templates/employee_template.xlsx
+++ b/public/templates/employee_template.xlsx
@@ -7,7 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Data Karyawan" sheetId="1" r:id="rId4"/>
+    <sheet name="Keterangan" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,53 +16,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
   <si>
     <t>nip</t>
   </si>
   <si>
+    <t>NIP</t>
+  </si>
+  <si>
     <t>nik</t>
   </si>
   <si>
+    <t>NIK</t>
+  </si>
+  <si>
     <t>nama_lengkap</t>
   </si>
   <si>
+    <t>Nama Lengkap</t>
+  </si>
+  <si>
     <t>nama_gelar</t>
   </si>
   <si>
+    <t>Nama Gelar</t>
+  </si>
+  <si>
     <t>jenis_kelamin</t>
   </si>
   <si>
+    <t>Jenis Kelamin (L/P)</t>
+  </si>
+  <si>
+    <t>tempat_lahir</t>
+  </si>
+  <si>
+    <t>Tempat Lahir</t>
+  </si>
+  <si>
+    <t>tanggal_lahir</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>status_pernikahan</t>
+  </si>
+  <si>
+    <t>Status Pernikahan</t>
+  </si>
+  <si>
+    <t>golongan_darah</t>
+  </si>
+  <si>
+    <t>Golongan Darah</t>
+  </si>
+  <si>
     <t>no_hp</t>
   </si>
   <si>
+    <t>No. HP</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>alamat</t>
   </si>
   <si>
+    <t>Alamat</t>
+  </si>
+  <si>
     <t>pendidikan_terakhir</t>
   </si>
   <si>
+    <t>Pendidikan Terakhir</t>
+  </si>
+  <si>
     <t>nomor_ijazah</t>
   </si>
   <si>
+    <t>Nomor Ijazah</t>
+  </si>
+  <si>
     <t>tahun_lulus_ijazah</t>
   </si>
   <si>
+    <t>Tahun Lulus</t>
+  </si>
+  <si>
     <t>jabatan</t>
   </si>
   <si>
+    <t>Jabatan</t>
+  </si>
+  <si>
     <t>unit</t>
   </si>
   <si>
+    <t>Unit</t>
+  </si>
+  <si>
     <t>tmt_sip</t>
   </si>
   <si>
+    <t>TMT SIP (YYYY-MM-DD)</t>
+  </si>
+  <si>
     <t>tat_sip</t>
   </si>
   <si>
+    <t>TAT SIP (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>19850101001</t>
+  </si>
+  <si>
+    <t>3201010185001001</t>
+  </si>
+  <si>
     <t>Budi Santoso</t>
   </si>
   <si>
@@ -71,6 +147,18 @@
     <t>L</t>
   </si>
   <si>
+    <t>Bukittinggi</t>
+  </si>
+  <si>
+    <t>1985-01-01</t>
+  </si>
+  <si>
+    <t>menikah</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
     <t>08123456789</t>
   </si>
   <si>
@@ -86,6 +174,9 @@
     <t>IJZ-001/2020</t>
   </si>
   <si>
+    <t>2020</t>
+  </si>
+  <si>
     <t>Dokter Umum</t>
   </si>
   <si>
@@ -96,6 +187,93 @@
   </si>
   <si>
     <t>2027-01-01</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Contoh / Pilihan</t>
+  </si>
+  <si>
+    <t>Nomor Induk Pegawai</t>
+  </si>
+  <si>
+    <t>NIK KTP 16 digit</t>
+  </si>
+  <si>
+    <t>Nama tanpa gelar</t>
+  </si>
+  <si>
+    <t>Gelar akademik</t>
+  </si>
+  <si>
+    <t>dr. / S.Kep. / S.Kom</t>
+  </si>
+  <si>
+    <t>Huruf kapital</t>
+  </si>
+  <si>
+    <t>L atau P</t>
+  </si>
+  <si>
+    <t>Kota kelahiran</t>
+  </si>
+  <si>
+    <t>Format YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Pilih salah satu</t>
+  </si>
+  <si>
+    <t>belum_menikah / menikah / cerai_hidup / cerai_mati</t>
+  </si>
+  <si>
+    <t>A / B / AB / O / A+ / A- / B+ / B- / AB+ / AB- / O+ / O-</t>
+  </si>
+  <si>
+    <t>Nomor WhatsApp aktif</t>
+  </si>
+  <si>
+    <t>Email aktif</t>
+  </si>
+  <si>
+    <t>nama@email.com</t>
+  </si>
+  <si>
+    <t>Alamat lengkap</t>
+  </si>
+  <si>
+    <t>Jl. Nama No. 1, Kota</t>
+  </si>
+  <si>
+    <t>SMA/SMK / D3 / D4 / S1 / S2 / S3 / Profesi</t>
+  </si>
+  <si>
+    <t>Nomor ijazah terakhir</t>
+  </si>
+  <si>
+    <t>4 digit tahun</t>
+  </si>
+  <si>
+    <t>Jabatan di RS</t>
+  </si>
+  <si>
+    <t>Dokter Umum / Perawat</t>
+  </si>
+  <si>
+    <t>Unit/Departemen</t>
+  </si>
+  <si>
+    <t>IGD / ICU / Poli Umum</t>
+  </si>
+  <si>
+    <t>Tanggal Mulai Tugas SIP</t>
+  </si>
+  <si>
+    <t>Tanggal Akhir Tugas SIP</t>
   </si>
 </sst>
 </file>
@@ -103,7 +281,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -118,12 +296,30 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,12 +328,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
+        <fgColor rgb="FF1F3864"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,13 +353,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,123 +682,465 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="O1" sqref="O1"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="true" style="0"/>
-    <col min="2" max="2" width="20" customWidth="true" style="0"/>
-    <col min="3" max="3" width="20" customWidth="true" style="0"/>
-    <col min="4" max="4" width="20" customWidth="true" style="0"/>
-    <col min="5" max="5" width="20" customWidth="true" style="0"/>
-    <col min="6" max="6" width="20" customWidth="true" style="0"/>
-    <col min="7" max="7" width="20" customWidth="true" style="0"/>
-    <col min="8" max="8" width="20" customWidth="true" style="0"/>
-    <col min="9" max="9" width="20" customWidth="true" style="0"/>
-    <col min="10" max="10" width="20" customWidth="true" style="0"/>
-    <col min="11" max="11" width="20" customWidth="true" style="0"/>
-    <col min="12" max="12" width="20" customWidth="true" style="0"/>
-    <col min="13" max="13" width="20" customWidth="true" style="0"/>
-    <col min="14" max="14" width="20" customWidth="true" style="0"/>
-    <col min="15" max="15" width="20" customWidth="true" style="0"/>
+    <col min="1" max="1" width="22" customWidth="true" style="0"/>
+    <col min="2" max="2" width="22" customWidth="true" style="0"/>
+    <col min="3" max="3" width="22" customWidth="true" style="0"/>
+    <col min="4" max="4" width="22" customWidth="true" style="0"/>
+    <col min="5" max="5" width="22" customWidth="true" style="0"/>
+    <col min="6" max="6" width="22" customWidth="true" style="0"/>
+    <col min="7" max="7" width="22" customWidth="true" style="0"/>
+    <col min="8" max="8" width="22" customWidth="true" style="0"/>
+    <col min="9" max="9" width="22" customWidth="true" style="0"/>
+    <col min="10" max="10" width="22" customWidth="true" style="0"/>
+    <col min="11" max="11" width="22" customWidth="true" style="0"/>
+    <col min="12" max="12" width="22" customWidth="true" style="0"/>
+    <col min="13" max="13" width="22" customWidth="true" style="0"/>
+    <col min="14" max="14" width="22" customWidth="true" style="0"/>
+    <col min="15" max="15" width="22" customWidth="true" style="0"/>
+    <col min="16" max="16" width="22" customWidth="true" style="0"/>
+    <col min="17" max="17" width="22" customWidth="true" style="0"/>
+    <col min="18" max="18" width="22" customWidth="true" style="0"/>
+    <col min="19" max="19" width="22" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19" customHeight="1" ht="20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" customHeight="1" ht="30">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" customHeight="1" ht="20">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1:C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="true" style="0"/>
+    <col min="2" max="2" width="30" customWidth="true" style="0"/>
+    <col min="3" max="3" width="55" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5">
+        <v>19850101001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3201010185001001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2">
-        <v>19850101001</v>
-      </c>
-      <c r="B2">
-        <v>3201010185001001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="B12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2">
+      <c r="B13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="5">
         <v>2020</v>
       </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: field data karyawan (golongan, tmt pns, agama)
</commit_message>
<xml_diff>
--- a/public/templates/employee_template.xlsx
+++ b/public/templates/employee_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>nip</t>
   </si>
@@ -72,6 +72,12 @@
     <t>Golongan Darah</t>
   </si>
   <si>
+    <t>agama</t>
+  </si>
+  <si>
+    <t>Agama</t>
+  </si>
+  <si>
     <t>no_hp</t>
   </si>
   <si>
@@ -96,6 +102,12 @@
     <t>Pendidikan Terakhir</t>
   </si>
   <si>
+    <t>prodi_pendidikan</t>
+  </si>
+  <si>
+    <t>Program Studi</t>
+  </si>
+  <si>
     <t>nomor_ijazah</t>
   </si>
   <si>
@@ -120,6 +132,18 @@
     <t>Unit</t>
   </si>
   <si>
+    <t>golongan_ruang</t>
+  </si>
+  <si>
+    <t>Golongan Ruang</t>
+  </si>
+  <si>
+    <t>tmt_pns</t>
+  </si>
+  <si>
+    <t>TMT PNS (YYYY-MM-DD)</t>
+  </si>
+  <si>
     <t>tmt_sip</t>
   </si>
   <si>
@@ -141,7 +165,7 @@
     <t>Budi Santoso</t>
   </si>
   <si>
-    <t>dr.</t>
+    <t>dr.Budi Santoso</t>
   </si>
   <si>
     <t>L</t>
@@ -210,7 +234,7 @@
     <t>Gelar akademik</t>
   </si>
   <si>
-    <t>dr. / S.Kep. / S.Kom</t>
+    <t>dr. Budi Santoso</t>
   </si>
   <si>
     <t>Huruf kapital</t>
@@ -381,8 +405,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,11 +706,11 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1:S3"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -710,9 +734,13 @@
     <col min="17" max="17" width="22" customWidth="true" style="0"/>
     <col min="18" max="18" width="22" customWidth="true" style="0"/>
     <col min="19" max="19" width="22" customWidth="true" style="0"/>
+    <col min="20" max="20" width="22" customWidth="true" style="0"/>
+    <col min="21" max="21" width="22" customWidth="true" style="0"/>
+    <col min="22" max="22" width="22" customWidth="true" style="0"/>
+    <col min="23" max="23" width="22" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" customHeight="1" ht="20">
+    <row r="1" spans="1:23" customHeight="1" ht="20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,8 +798,20 @@
       <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" customHeight="1" ht="30">
+      <c r="T1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" customHeight="1" ht="30">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -829,65 +869,81 @@
       <c r="S2" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" customHeight="1" ht="20">
+      <c r="T2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" customHeight="1" ht="20">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -924,223 +980,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="4">
+        <v>19850101001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3201010185001001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="5">
-        <v>19850101001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="5">
-        <v>3201010185001001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>